<commit_message>
Prueba de grafico con matplotlib
Agregue las coordenadas de cada capital
</commit_message>
<xml_diff>
--- a/Ejercicio3/TablaCapitales.xlsx
+++ b/Ejercicio3/TablaCapitales.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\AlgoritmosGeneticos\Ejercicio3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzaccaro\PycharmProjects\AlgoritmosGeneticos\Ejercicio3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED99B5DD-1064-498E-9AA3-9629B6B530A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Coordenadas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="290">
   <si>
     <t>Distancias en kilómetros</t>
   </si>
@@ -902,12 +904,21 @@
   <si>
     <t>1605</t>
   </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -935,6 +946,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF4299E1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1021,10 +1053,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1056,8 +1089,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1335,10 +1372,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y955"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4158,4 +4197,315 @@
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA40DCD4-8D90-472D-A2E8-C6B6E746AEAA}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>-34.613149999999997</v>
+      </c>
+      <c r="C2" s="11">
+        <v>-58.377229999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>-31.413499999999999</v>
+      </c>
+      <c r="C3" s="11">
+        <v>-64.181049999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>-27.467839999999999</v>
+      </c>
+      <c r="C4" s="12">
+        <v>-58.834400000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>-26.184889999999999</v>
+      </c>
+      <c r="C5" s="12">
+        <v>-58.17313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>-34.92145</v>
+      </c>
+      <c r="C6" s="11">
+        <v>-57.954529999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>-29.411049999999999</v>
+      </c>
+      <c r="C7" s="12">
+        <v>-66.850669999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>-32.890839999999997</v>
+      </c>
+      <c r="C8" s="12">
+        <v>-68.827169999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>-38.951610000000002</v>
+      </c>
+      <c r="C9" s="12">
+        <v>-68.059100000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>-31.732710000000001</v>
+      </c>
+      <c r="C10" s="11">
+        <v>-60.528970000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>-27.367080000000001</v>
+      </c>
+      <c r="C11" s="11">
+        <v>-55.896079999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>-43.300159999999998</v>
+      </c>
+      <c r="C12" s="12">
+        <v>-65.102279999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="12">
+        <v>-27.460560000000001</v>
+      </c>
+      <c r="C13" s="12">
+        <v>-58.983890000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="12">
+        <v>-51.622610000000002</v>
+      </c>
+      <c r="C14" s="12">
+        <v>-69.218130000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
+        <v>-28.469570000000001</v>
+      </c>
+      <c r="C15" s="12">
+        <v>-65.785240000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12">
+        <v>-26.82414</v>
+      </c>
+      <c r="C16" s="12">
+        <v>-65.2226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="12">
+        <v>-24.194569999999999</v>
+      </c>
+      <c r="C17" s="12">
+        <v>-65.297120000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12">
+        <v>-24.785900000000002</v>
+      </c>
+      <c r="C18" s="12">
+        <v>-65.411659999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11">
+        <v>-31.537500000000001</v>
+      </c>
+      <c r="C19" s="11">
+        <v>-68.536389999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12">
+        <v>-33.295009999999998</v>
+      </c>
+      <c r="C20" s="12">
+        <v>-66.335629999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11">
+        <v>-31.648810000000001</v>
+      </c>
+      <c r="C21" s="11">
+        <v>-60.708680000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12">
+        <v>-36.616669999999999</v>
+      </c>
+      <c r="C22" s="12">
+        <v>-64.283330000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12">
+        <v>-27.795110000000001</v>
+      </c>
+      <c r="C23" s="12">
+        <v>-64.261489999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12">
+        <v>-54.810839999999999</v>
+      </c>
+      <c r="C24" s="12">
+        <v>-68.315910000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="12">
+        <v>-40.813450000000003</v>
+      </c>
+      <c r="C25" s="12">
+        <v>-62.996679999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.geodatos.net/coordenadas/argentina/buenos-aires" xr:uid="{93918FB1-4914-428A-8791-44B2441C370F}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://www.geodatos.net/coordenadas/argentina/buenos-aires" xr:uid="{804F9407-3B72-4DF1-AED8-5DB9FB17A3F7}"/>
+    <hyperlink ref="B3" r:id="rId3" display="https://www.geodatos.net/coordenadas/argentina/cordoba" xr:uid="{9D93C1AA-9B2F-4C31-80A2-A7F476A033C7}"/>
+    <hyperlink ref="C3" r:id="rId4" display="https://www.geodatos.net/coordenadas/argentina/cordoba" xr:uid="{0205A84E-BFB9-4EBE-B911-55473432DCA4}"/>
+    <hyperlink ref="B21" r:id="rId5" display="https://www.geodatos.net/coordenadas/argentina/santa-fe" xr:uid="{DFD3B230-47A8-46BC-B818-5CBFA7B797AA}"/>
+    <hyperlink ref="C21" r:id="rId6" display="https://www.geodatos.net/coordenadas/argentina/santa-fe" xr:uid="{9296EDAE-F691-4521-9D69-91B908899E4B}"/>
+    <hyperlink ref="B19" r:id="rId7" display="https://www.geodatos.net/coordenadas/argentina/san-juan" xr:uid="{7974BB98-BC45-4226-98DE-F6414321805F}"/>
+    <hyperlink ref="C19" r:id="rId8" display="https://www.geodatos.net/coordenadas/argentina/san-juan" xr:uid="{B4EC36BE-3DD9-4A50-96E5-DD1F3A83EF80}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.geodatos.net/coordenadas/argentina/parana" xr:uid="{C5AEB384-CCB3-49ED-89A9-AAEC711588D4}"/>
+    <hyperlink ref="C10" r:id="rId10" display="https://www.geodatos.net/coordenadas/argentina/parana" xr:uid="{2225DB58-3A79-4F3C-B6C4-780772F543BE}"/>
+    <hyperlink ref="B11" r:id="rId11" display="https://www.geodatos.net/coordenadas/argentina/posadas" xr:uid="{4022C993-48B8-442A-B85E-91AC8584CF15}"/>
+    <hyperlink ref="C11" r:id="rId12" display="https://www.geodatos.net/coordenadas/argentina/posadas" xr:uid="{17421CAF-B340-42B5-868F-DD8F128F834F}"/>
+    <hyperlink ref="B6" r:id="rId13" display="https://www.geodatos.net/coordenadas/argentina/la-plata" xr:uid="{ED922103-5072-4DF3-AC34-8F8333292132}"/>
+    <hyperlink ref="C6" r:id="rId14" display="https://www.geodatos.net/coordenadas/argentina/la-plata" xr:uid="{869CE5E4-E381-4A0A-BDA5-521ED3ECB168}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lectura de datos de excel para mapa implementada
</commit_message>
<xml_diff>
--- a/Ejercicio3/TablaCapitales.xlsx
+++ b/Ejercicio3/TablaCapitales.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Apuntes UTN\III\Algoritmos Genéticos\TPs\Ejercicio3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6D9985-CF81-4796-AEEE-FB348916B85B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8355" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="29160" yWindow="1530" windowWidth="21600" windowHeight="11835" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="289">
   <si>
     <t>Distancias en kilómetros</t>
   </si>
@@ -903,14 +909,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="27">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -960,345 +960,16 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1373,249 +1044,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1623,7 +1055,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1653,61 +1085,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1965,12 +1354,12 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y955"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -1979,14 +1368,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.8857142857143" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="14.7142857142857" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="25" width="13" customWidth="1"/>
-    <col min="26" max="1005" width="14.4380952380952" customWidth="1"/>
+    <col min="26" max="1005" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46.5" customHeight="1" spans="1:25">
+    <row r="1" spans="1:25" ht="46.5" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +1452,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:25">
+    <row r="2" spans="1:25" ht="16.5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2138,7 +1527,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" ht="17.25" spans="1:25">
+    <row r="3" spans="1:25" ht="16.5">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -2213,7 +1602,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" ht="17.25" spans="1:25">
+    <row r="4" spans="1:25" ht="16.5">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -2288,7 +1677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" ht="17.25" spans="1:25">
+    <row r="5" spans="1:25" ht="16.5">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +1752,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" ht="17.25" spans="1:25">
+    <row r="6" spans="1:25" ht="16.5">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2438,7 +1827,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" ht="17.25" spans="1:25">
+    <row r="7" spans="1:25" ht="16.5">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -2513,7 +1902,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" ht="17.25" spans="1:25">
+    <row r="8" spans="1:25" ht="16.5">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -2588,7 +1977,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" ht="17.25" spans="1:25">
+    <row r="9" spans="1:25" ht="16.5">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -2663,7 +2052,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" ht="17.25" spans="1:25">
+    <row r="10" spans="1:25" ht="16.5">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2738,7 +2127,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" ht="17.25" spans="1:25">
+    <row r="11" spans="1:25" ht="16.5">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2813,7 +2202,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" ht="17.25" spans="1:25">
+    <row r="12" spans="1:25" ht="16.5">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -2888,7 +2277,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" ht="17.25" spans="1:25">
+    <row r="13" spans="1:25" ht="16.5">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -2963,7 +2352,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" ht="17.25" spans="1:25">
+    <row r="14" spans="1:25" ht="16.5">
       <c r="A14" s="4" t="s">
         <v>223</v>
       </c>
@@ -3038,7 +2427,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" ht="17.25" spans="1:25">
+    <row r="15" spans="1:25" ht="16.5">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
@@ -3113,7 +2502,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="16" ht="17.25" spans="1:25">
+    <row r="16" spans="1:25" ht="16.5">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -3188,7 +2577,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="17" ht="17.25" spans="1:25">
+    <row r="17" spans="1:25" ht="16.5">
       <c r="A17" s="4" t="s">
         <v>252</v>
       </c>
@@ -3263,7 +2652,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" ht="17.25" spans="1:25">
+    <row r="18" spans="1:25" ht="16.5">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -3338,7 +2727,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="19" ht="17.25" spans="1:25">
+    <row r="19" spans="1:25" ht="16.5">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -3413,7 +2802,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" ht="17.25" spans="1:25">
+    <row r="20" spans="1:25" ht="16.5">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -3488,7 +2877,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:25">
+    <row r="21" spans="1:25" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -3563,7 +2952,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:25">
+    <row r="22" spans="1:25" ht="15.75" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -3638,7 +3027,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:25">
+    <row r="23" spans="1:25" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -3713,7 +3102,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:25">
+    <row r="24" spans="1:25" ht="15.75" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>23</v>
       </c>
@@ -3788,7 +3177,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:25">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
@@ -3863,13 +3252,13 @@
       </c>
       <c r="Y25" s="13"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:25" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -4794,28 +4183,26 @@
     <row r="954" ht="15.75" customHeight="1"/>
     <row r="955" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.510416666666667" footer="0.510416666666667"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.552380952381" customWidth="1"/>
-    <col min="2" max="3" width="10.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5" spans="1:3">
+    <row r="1" spans="1:3" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>286</v>
       </c>
@@ -4826,289 +4213,272 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" ht="17.25" spans="1:3">
+    <row r="2" spans="1:3" ht="16.5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>-34.61315</v>
+        <v>354</v>
       </c>
       <c r="C2" s="3">
-        <v>-58.37723</v>
-      </c>
-    </row>
-    <row r="3" ht="17.25" spans="1:3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>-31.4135</v>
+        <v>238</v>
       </c>
       <c r="C3" s="3">
-        <v>-64.18105</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" spans="1:3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>-27.46784</v>
+        <v>349</v>
       </c>
       <c r="C4" s="5">
-        <v>-58.8344</v>
-      </c>
-    </row>
-    <row r="5" ht="17.25" spans="1:3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>-26.18489</v>
+        <v>357</v>
       </c>
       <c r="C5" s="5">
-        <v>-58.17313</v>
-      </c>
-    </row>
-    <row r="6" ht="17.25" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>-34.92145</v>
+        <v>365</v>
       </c>
       <c r="C6" s="3">
-        <v>-57.95453</v>
-      </c>
-    </row>
-    <row r="7" ht="17.25" spans="1:3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>-29.41105</v>
+        <v>172</v>
       </c>
       <c r="C7" s="5">
-        <v>-66.85067</v>
-      </c>
-    </row>
-    <row r="8" ht="17.25" spans="1:3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>-32.89084</v>
+        <v>128</v>
       </c>
       <c r="C8" s="5">
-        <v>-68.82717</v>
-      </c>
-    </row>
-    <row r="9" ht="17.25" spans="1:3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.25">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>-38.95161</v>
+        <v>139</v>
       </c>
       <c r="C9" s="5">
-        <v>-68.0591</v>
-      </c>
-    </row>
-    <row r="10" ht="17.25" spans="1:3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>-31.73271</v>
+        <v>312</v>
       </c>
       <c r="C10" s="3">
-        <v>-60.52897</v>
-      </c>
-    </row>
-    <row r="11" ht="17.25" spans="1:3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>-27.36708</v>
+        <v>411</v>
       </c>
       <c r="C11" s="3">
-        <v>-55.89608</v>
-      </c>
-    </row>
-    <row r="12" ht="17.25" spans="1:3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>-43.30016</v>
+        <v>210</v>
       </c>
       <c r="C12" s="5">
-        <v>-65.10228</v>
-      </c>
-    </row>
-    <row r="13" ht="17.25" spans="1:3">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>-27.46056</v>
+        <v>341</v>
       </c>
       <c r="C13" s="5">
-        <v>-58.98389</v>
-      </c>
-    </row>
-    <row r="14" ht="17.25" spans="1:3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17.25">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="5">
-        <v>-51.62261</v>
+        <v>117</v>
       </c>
       <c r="C14" s="5">
-        <v>-69.21813</v>
-      </c>
-    </row>
-    <row r="15" ht="17.25" spans="1:3">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17.25">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="5">
-        <v>-28.46957</v>
+        <v>194</v>
       </c>
       <c r="C15" s="5">
-        <v>-65.78524</v>
-      </c>
-    </row>
-    <row r="16" ht="17.25" spans="1:3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17.25">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="5">
-        <v>-26.82414</v>
+        <v>203</v>
       </c>
       <c r="C16" s="5">
-        <v>-65.2226</v>
-      </c>
-    </row>
-    <row r="17" ht="17.25" spans="1:3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25">
       <c r="A17" s="4" t="s">
         <v>252</v>
       </c>
       <c r="B17" s="5">
-        <v>-24.19457</v>
+        <v>203</v>
       </c>
       <c r="C17" s="5">
-        <v>-65.29712</v>
-      </c>
-    </row>
-    <row r="18" ht="17.25" spans="1:3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="5">
-        <v>-24.7859</v>
+        <v>203</v>
       </c>
       <c r="C18" s="5">
-        <v>-65.41166</v>
-      </c>
-    </row>
-    <row r="19" ht="17.25" spans="1:3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16.5">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>-31.5375</v>
+        <v>133</v>
       </c>
       <c r="C19" s="3">
-        <v>-68.53639</v>
-      </c>
-    </row>
-    <row r="20" ht="17.25" spans="1:3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.25">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="5">
-        <v>-33.29501</v>
+        <v>178</v>
       </c>
       <c r="C20" s="5">
-        <v>-66.33563</v>
-      </c>
-    </row>
-    <row r="21" ht="17.25" spans="1:3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>-31.64881</v>
+        <v>303</v>
       </c>
       <c r="C21" s="3">
-        <v>-60.70868</v>
-      </c>
-    </row>
-    <row r="22" ht="17.25" spans="1:3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="5">
-        <v>-36.61667</v>
+        <v>228</v>
       </c>
       <c r="C22" s="5">
-        <v>-64.28333</v>
-      </c>
-    </row>
-    <row r="23" ht="17.25" spans="1:3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.25">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="5">
-        <v>-27.79511</v>
+        <v>224</v>
       </c>
       <c r="C23" s="5">
-        <v>-64.26149</v>
-      </c>
-    </row>
-    <row r="24" ht="17.25" spans="1:3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17.25">
       <c r="A24" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="5">
-        <v>-54.81084</v>
+        <v>139</v>
       </c>
       <c r="C24" s="5">
-        <v>-68.31591</v>
-      </c>
-    </row>
-    <row r="25" ht="17.25" spans="1:3">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17.25">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="5">
-        <v>-40.81345</v>
+        <v>250</v>
       </c>
       <c r="C25" s="5">
-        <v>-62.99668</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="-34,61315"/>
-    <hyperlink ref="C2" r:id="rId1" display="-58,37723"/>
-    <hyperlink ref="B3" r:id="rId2" display="-31,4135"/>
-    <hyperlink ref="C3" r:id="rId2" display="-64,18105"/>
-    <hyperlink ref="B21" r:id="rId3" display="-31,64881"/>
-    <hyperlink ref="C21" r:id="rId3" display="-60,70868"/>
-    <hyperlink ref="B19" r:id="rId4" display="-31,5375"/>
-    <hyperlink ref="C19" r:id="rId4" display="-68,53639"/>
-    <hyperlink ref="B10" r:id="rId5" display="-31,73271"/>
-    <hyperlink ref="C10" r:id="rId5" display="-60,52897"/>
-    <hyperlink ref="B11" r:id="rId6" display="-27,36708"/>
-    <hyperlink ref="C11" r:id="rId6" display="-55,89608"/>
-    <hyperlink ref="B6" r:id="rId7" display="-34,92145"/>
-    <hyperlink ref="C6" r:id="rId7" display="-57,95453"/>
-  </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>